<commit_message>
neural network for 6 nimmt - use learning curve to define sample volumn
</commit_message>
<xml_diff>
--- a/40_Python/20231022_6Nimmt/模型参数.xlsx
+++ b/40_Python/20231022_6Nimmt/模型参数.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\Marvin_Haves_Fun_2309\40_Python\20231022_6Nimmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C79B88-C6F3-4489-AFF7-B80EC24A0AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D370C1-16E7-43F7-B873-755E2914100C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="模型参数" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="参数总量" sheetId="2" r:id="rId2"/>
+    <sheet name="学习曲线" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -196,6 +197,42 @@
   </si>
   <si>
     <t>model_12.pth</t>
+  </si>
+  <si>
+    <t>训练集</t>
+  </si>
+  <si>
+    <t>start_index</t>
+  </si>
+  <si>
+    <t>end_index</t>
+  </si>
+  <si>
+    <t>测试集</t>
+  </si>
+  <si>
+    <t>MSE-epoch2000</t>
+  </si>
+  <si>
+    <t>MSE-epoch1000</t>
+  </si>
+  <si>
+    <t>固定的</t>
+  </si>
+  <si>
+    <t>10000局游戏</t>
+  </si>
+  <si>
+    <t>epoch=20000，没啥用</t>
+  </si>
+  <si>
+    <t>训练误差</t>
+  </si>
+  <si>
+    <t>测试误差</t>
+  </si>
+  <si>
+    <t>MSE-测试</t>
   </si>
 </sst>
 </file>
@@ -520,7 +557,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -650,6 +687,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -695,7 +743,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -715,6 +763,9 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -828,7 +879,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$1</c:f>
+              <c:f>参数总量!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -851,7 +902,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$102</c:f>
+              <c:f>参数总量!$A$2:$A$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -1160,7 +1211,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$102</c:f>
+              <c:f>参数总量!$N$2:$N$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -1479,7 +1530,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$1</c:f>
+              <c:f>参数总量!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1502,7 +1553,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$102</c:f>
+              <c:f>参数总量!$A$2:$A$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -1811,7 +1862,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$102</c:f>
+              <c:f>参数总量!$O$2:$O$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -2130,7 +2181,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$1</c:f>
+              <c:f>参数总量!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2153,7 +2204,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$102</c:f>
+              <c:f>参数总量!$A$2:$A$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -2462,7 +2513,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$102</c:f>
+              <c:f>参数总量!$P$2:$P$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -2781,7 +2832,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$1</c:f>
+              <c:f>参数总量!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2804,7 +2855,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$102</c:f>
+              <c:f>参数总量!$A$2:$A$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -3113,7 +3164,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$102</c:f>
+              <c:f>参数总量!$Q$2:$Q$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -3629,6 +3680,573 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>学习曲线!$H$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSE-epoch1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>学习曲线!$E$8:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>学习曲线!$H$8:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.1999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0088999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1187</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9344000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1806999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0553999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1404000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3973</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9AC3-4939-83D9-8F387C173630}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>学习曲线!$I$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSE-epoch2000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>学习曲线!$E$8:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>学习曲线!$I$8:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89849999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9575</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3536000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4685999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8096000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6467000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0137999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1745000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9AC3-4939-83D9-8F387C173630}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>学习曲线!$J$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSE-测试</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>学习曲线!$E$8:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>学习曲线!$J$8:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>13.410245</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.055565</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.740119</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2213079999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7513350000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0742269999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2015120000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7499319999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7408459999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9AC3-4939-83D9-8F387C173630}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1649470736"/>
+        <c:axId val="340994928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1649470736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="340994928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="340994928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1649470736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3669,7 +4287,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4226,6 +5400,91 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>56468</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>17145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD2C98D3-D77B-579D-1454-1C514407639C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2914650"/>
+          <a:ext cx="6714443" cy="3114675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>112394</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>141921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29E7251D-ED48-1B80-C7B2-2CDC1EBC061A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4526,7 +5785,7 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4591,6 +5850,9 @@
       </c>
       <c r="Q1" s="10" t="s">
         <v>32</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -5438,13 +6700,13 @@
       <c r="N20" s="2">
         <v>45389</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="9">
         <v>4.0131730000000001</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20" s="21">
         <v>0.38844000000000001</v>
       </c>
-      <c r="Q20" s="8">
+      <c r="Q20" s="21">
         <v>0.67800000000000005</v>
       </c>
     </row>
@@ -5456,6 +6718,15 @@
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
       <c r="N21" s="18"/>
+      <c r="O21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P21" s="21">
+        <v>0.39951999999999999</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>0.64100000000000001</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -5615,7 +6886,7 @@
   <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N42" sqref="N42:Q102"/>
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12400,4 +13671,377 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EADD6BF-BAE1-4929-B3C4-C61A1CFF22B4}">
+  <dimension ref="A1:Q16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1">
+        <v>54</v>
+      </c>
+      <c r="C2" s="4">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <f t="shared" ref="H2" si="0">(B2+1)*C2+(C2+1)*G2</f>
+        <v>673</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K2" s="4">
+        <v>2001</v>
+      </c>
+      <c r="L2" s="1">
+        <v>8000</v>
+      </c>
+      <c r="M2" s="5">
+        <v>4</v>
+      </c>
+      <c r="N2" s="2">
+        <v>45389</v>
+      </c>
+      <c r="O2">
+        <v>4.0131730000000001</v>
+      </c>
+      <c r="P2" s="8">
+        <v>0.38844000000000001</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>0.67800000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>60000</v>
+      </c>
+      <c r="B8" s="19">
+        <v>61000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>100</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="J8" s="1">
+        <v>13.410245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>500</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>1.0088999999999999</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.89849999999999997</v>
+      </c>
+      <c r="J9" s="1">
+        <v>12.055565</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>2.1187</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1.9575</v>
+      </c>
+      <c r="J10" s="1">
+        <v>6.740119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>2.5238</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2.3536000000000001</v>
+      </c>
+      <c r="J11" s="1">
+        <v>5.2213079999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>2.9344000000000001</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2.4685999999999999</v>
+      </c>
+      <c r="J12" s="1">
+        <v>4.7513350000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <v>8000</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6">
+        <v>3.1806999999999999</v>
+      </c>
+      <c r="I13" s="6">
+        <v>2.8096000000000001</v>
+      </c>
+      <c r="J13" s="6">
+        <v>4.0742269999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>12000</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1">
+        <v>4.0553999999999997</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3.6467000000000001</v>
+      </c>
+      <c r="J14" s="1">
+        <v>4.2015120000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>16000</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1">
+        <v>3.1404000000000001</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3.0137999999999998</v>
+      </c>
+      <c r="J15" s="1">
+        <v>3.7499319999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>20000</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1">
+        <v>3.3973</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3.1745000000000001</v>
+      </c>
+      <c r="J16" s="1">
+        <v>3.7408459999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>